<commit_message>
Optimized the code in finding violations and plate numbers
</commit_message>
<xml_diff>
--- a/dat/Violation-Database.xlsx
+++ b/dat/Violation-Database.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>DATE</t>
   </si>
@@ -65,9 +65,6 @@
     <t>5:26pm</t>
   </si>
   <si>
-    <t>zxy</t>
-  </si>
-  <si>
     <t>truck</t>
   </si>
   <si>
@@ -78,6 +75,12 @@
   </si>
   <si>
     <t>12:00nn</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>January 10, 2016</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +529,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -536,7 +556,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,19 +586,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -591,7 +611,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
improved ways of searching
</commit_message>
<xml_diff>
--- a/dat/Violation-Database.xlsx
+++ b/dat/Violation-Database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SPEEDING" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="DRUNK DRIVING" sheetId="3" r:id="rId3"/>
     <sheet name="COUNTERFLOWING" sheetId="4" r:id="rId4"/>
     <sheet name="BEATING THE RED LIGHT" sheetId="5" r:id="rId5"/>
+    <sheet name="COLOR CODING" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
   <si>
     <t>DATE</t>
   </si>
@@ -71,16 +72,37 @@
     <t>black</t>
   </si>
   <si>
-    <t>December 12, 2013</t>
-  </si>
-  <si>
-    <t>12:00nn</t>
-  </si>
-  <si>
     <t>xyz</t>
   </si>
   <si>
     <t>January 10, 2016</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Jan 12, 2015</t>
+  </si>
+  <si>
+    <t>12:00NN</t>
+  </si>
+  <si>
+    <t>Dec 13, 2016</t>
+  </si>
+  <si>
+    <t>11:00AM</t>
+  </si>
+  <si>
+    <t>July 3, 2016</t>
+  </si>
+  <si>
+    <t>3:00am</t>
+  </si>
+  <si>
+    <t>November 3, 2016</t>
+  </si>
+  <si>
+    <t>September 3, 2016</t>
   </si>
 </sst>
 </file>
@@ -420,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +512,23 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -500,7 +539,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +570,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -540,10 +579,10 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -555,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -595,7 +634,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -608,10 +647,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,6 +678,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -649,7 +705,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,4 +737,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the searching result in showing all violations
</commit_message>
<xml_diff>
--- a/dat/Violation-Database.xlsx
+++ b/dat/Violation-Database.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\DLSU\5th Year 3rd Term\Syanade\Project\TraVIS-v1\dat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" tabRatio="679" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SPEEDING" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>DATE</t>
   </si>
@@ -87,12 +92,6 @@
     <t>12:00NN</t>
   </si>
   <si>
-    <t>Dec 13, 2016</t>
-  </si>
-  <si>
-    <t>11:00AM</t>
-  </si>
-  <si>
     <t>July 3, 2016</t>
   </si>
   <si>
@@ -103,12 +102,39 @@
   </si>
   <si>
     <t>September 3, 2016</t>
+  </si>
+  <si>
+    <t>suv</t>
+  </si>
+  <si>
+    <t>July 2, 2016</t>
+  </si>
+  <si>
+    <t>3:26pm</t>
+  </si>
+  <si>
+    <t>government</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>August 2, 2015</t>
+  </si>
+  <si>
+    <t>8:00am</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -150,6 +176,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -198,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,9 +260,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,6 +312,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,7 +508,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="A4:E4"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,10 +586,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -536,10 +599,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,10 +642,27 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -649,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -689,10 +769,10 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -702,10 +782,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,6 +814,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -741,10 +838,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,36 +872,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enlarged the height of the Graph
</commit_message>
<xml_diff>
--- a/dat/Violation-Database.xlsx
+++ b/dat/Violation-Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" tabRatio="679" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" tabRatio="679" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SPEEDING" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="COUNTERFLOWING" sheetId="4" r:id="rId5"/>
     <sheet name="BEATING THE RED LIGHT" sheetId="5" r:id="rId6"/>
     <sheet name="COLOR CODING" sheetId="6" r:id="rId7"/>
+    <sheet name="DRIVING ON SLIPPERS" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="30">
   <si>
     <t>DATE</t>
   </si>
@@ -587,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -917,7 +918,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,4 +967,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed the bug in About scene when speak button is not pressed. Finished added all the information needed in Facts scene. Excel Database was updated. (Location and Penalty Columns were added) Screenshot of about scene was added. Modified the content of about scene.
</commit_message>
<xml_diff>
--- a/dat/Violation-Database.xlsx
+++ b/dat/Violation-Database.xlsx
@@ -9,24 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" tabRatio="679" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520" tabRatio="679" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SPEEDING" sheetId="1" r:id="rId1"/>
     <sheet name="DRIVING WITHOUT LICENSE" sheetId="7" r:id="rId2"/>
-    <sheet name="SWERVING" sheetId="2" r:id="rId3"/>
+    <sheet name="NO SPARE TIRE" sheetId="2" r:id="rId3"/>
     <sheet name="DRUNK DRIVING" sheetId="3" r:id="rId4"/>
-    <sheet name="COUNTERFLOWING" sheetId="4" r:id="rId5"/>
+    <sheet name="OVERLOADING" sheetId="4" r:id="rId5"/>
     <sheet name="BEATING THE RED LIGHT" sheetId="5" r:id="rId6"/>
     <sheet name="COLOR CODING" sheetId="6" r:id="rId7"/>
-    <sheet name="DRIVING ON SLIPPERS" sheetId="9" r:id="rId8"/>
+    <sheet name="OVERNIGHT PARKING" sheetId="9" r:id="rId8"/>
+    <sheet name="SMOKE BELCHING" sheetId="11" r:id="rId9"/>
+    <sheet name="RECKLESS DRIVING" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="32">
   <si>
     <t>DATE</t>
   </si>
@@ -116,6 +118,12 @@
   </si>
   <si>
     <t>March 2, 2014</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>PENALTY</t>
   </si>
 </sst>
 </file>
@@ -492,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +519,7 @@
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -527,8 +535,14 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -545,7 +559,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -562,7 +576,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -584,12 +598,67 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,9 +668,11 @@
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -617,8 +688,14 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -635,7 +712,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -659,10 +736,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +751,7 @@
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -690,8 +767,14 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -708,7 +791,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -732,10 +815,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +829,7 @@
     <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -762,8 +845,14 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -787,10 +876,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +890,7 @@
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -817,8 +906,14 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -842,10 +937,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +952,7 @@
     <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -873,8 +968,14 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -891,7 +992,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -915,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E2"/>
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +1031,7 @@
     <col min="5" max="5" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -946,8 +1047,14 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -971,15 +1078,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -995,8 +1102,69 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>

</xml_diff>